<commit_message>
Corrected baseline with both
</commit_message>
<xml_diff>
--- a/Project/Results/SS340_Project_ResultsSummary.xlsx
+++ b/Project/Results/SS340_Project_ResultsSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared\.spyder-py3\SS340_Abdelwahed\Project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA632A61-EDA6-4C88-B5B5-22B9FCC42A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7798DF4A-29A1-4472-8A99-50BE03812AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="544" xr2:uid="{BD707416-7642-4DB3-9659-E87C42C0AA26}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>const</t>
   </si>
@@ -171,13 +171,16 @@
     <t>Baseline both</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.31) </t>
-  </si>
-  <si>
     <t>Heteroskedastically robust standard errors in parentheses.</t>
   </si>
   <si>
     <t>* p$&lt;$.1, ** p$&lt;$.05, ***p$&lt;$.01</t>
+  </si>
+  <si>
+    <t>-0.58***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.02) </t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +605,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -622,7 +625,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -821,7 +824,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -832,7 +835,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>